<commit_message>
added values to trait dataset, still playing with imputation
</commit_message>
<xml_diff>
--- a/data/traits/RF_trait_data2h.xlsx
+++ b/data/traits/RF_trait_data2h.xlsx
@@ -386,7 +386,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9175" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9349" uniqueCount="778">
   <si>
     <t>source</t>
   </si>
@@ -2705,6 +2705,36 @@
   </si>
   <si>
     <t>Carronia multisepalea</t>
+  </si>
+  <si>
+    <t>C. James SEQLD field data</t>
+  </si>
+  <si>
+    <t>Argyrodendron trifoliolatum</t>
+  </si>
+  <si>
+    <t>Ligustrum sinensis</t>
+  </si>
+  <si>
+    <t>Syzygium australae</t>
+  </si>
+  <si>
+    <t>Cupaniopsis anarcoides</t>
+  </si>
+  <si>
+    <t>Enidandra discolor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cryptocarya laevigata </t>
+  </si>
+  <si>
+    <t>Wilkea huegeliana</t>
+  </si>
+  <si>
+    <t>Sloenea australis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mm2/mg</t>
   </si>
 </sst>
 </file>
@@ -3897,11 +3927,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:P2442"/>
+  <dimension ref="A1:P2500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A907" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2214" sqref="A2214"/>
+      <pane ySplit="1" topLeftCell="A2488" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D802" sqref="D802"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -11897,7 +11927,7 @@
         <v>10.248996536267319</v>
       </c>
       <c r="C535" s="19" t="s">
-        <v>215</v>
+        <v>777</v>
       </c>
       <c r="D535" s="19"/>
       <c r="G535" s="25">
@@ -17302,7 +17332,7 @@
         <v>9.1944320689292809</v>
       </c>
       <c r="C908" s="19" t="s">
-        <v>215</v>
+        <v>777</v>
       </c>
       <c r="D908" s="19"/>
       <c r="G908" s="25">
@@ -18351,7 +18381,7 @@
         <v>11.978051664006619</v>
       </c>
       <c r="C978" s="19" t="s">
-        <v>215</v>
+        <v>777</v>
       </c>
       <c r="D978" s="19"/>
       <c r="G978" s="25">
@@ -18565,7 +18595,7 @@
         <v>9.2760419327842154</v>
       </c>
       <c r="C993" s="19" t="s">
-        <v>215</v>
+        <v>777</v>
       </c>
       <c r="D993" s="19"/>
       <c r="G993" s="25">
@@ -19736,7 +19766,7 @@
         <v>8.4203392270920929</v>
       </c>
       <c r="C1077" s="19" t="s">
-        <v>215</v>
+        <v>777</v>
       </c>
       <c r="D1077" s="19"/>
       <c r="G1077" s="25">
@@ -37538,6 +37568,992 @@
       </c>
       <c r="O2442" s="1" t="s">
         <v>765</v>
+      </c>
+    </row>
+    <row r="2443" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2443" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2443">
+        <v>158.60072042857101</v>
+      </c>
+      <c r="C2443" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2443">
+        <v>8.0011428571428596</v>
+      </c>
+      <c r="O2443" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2444" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2444" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2444">
+        <v>226.17794900000001</v>
+      </c>
+      <c r="C2444" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2444">
+        <v>28.468499999999999</v>
+      </c>
+      <c r="O2444" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2445" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2445" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2445">
+        <v>233.92141054999999</v>
+      </c>
+      <c r="C2445" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2445">
+        <v>13.7425</v>
+      </c>
+      <c r="O2445" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2446" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2446" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2446">
+        <v>129.94389029999999</v>
+      </c>
+      <c r="C2446" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2446">
+        <v>62.703000000000003</v>
+      </c>
+      <c r="O2446" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2447" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2447" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2447">
+        <v>209.09786993333299</v>
+      </c>
+      <c r="C2447" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2447">
+        <v>15.506166666666701</v>
+      </c>
+      <c r="O2447" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2448" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2448" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2448">
+        <v>191.17501100000001</v>
+      </c>
+      <c r="C2448" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2448">
+        <v>34.576999999999998</v>
+      </c>
+      <c r="O2448" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2449" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2449" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2449">
+        <v>114.8579689</v>
+      </c>
+      <c r="C2449" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2449">
+        <v>116.05200000000001</v>
+      </c>
+      <c r="O2449" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2450" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2450" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2450">
+        <v>206.97706769999999</v>
+      </c>
+      <c r="C2450" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2450">
+        <v>32.847000000000001</v>
+      </c>
+      <c r="O2450" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2451" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2451" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2451">
+        <v>248.8002098</v>
+      </c>
+      <c r="C2451" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2451">
+        <v>15.7783333333333</v>
+      </c>
+      <c r="O2451" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2452" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2452" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2452">
+        <v>183.08620970000001</v>
+      </c>
+      <c r="C2452" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2452">
+        <v>2.266</v>
+      </c>
+      <c r="O2452" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2453" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2453" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2453">
+        <v>217.14579685000001</v>
+      </c>
+      <c r="C2453" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2453">
+        <v>39.816000000000003</v>
+      </c>
+      <c r="O2453" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2454" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2454" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2454">
+        <v>77.831765509999997</v>
+      </c>
+      <c r="C2454" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2454">
+        <v>3.5350000000000001</v>
+      </c>
+      <c r="O2454" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2455" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2455" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2455">
+        <v>26.509235938749999</v>
+      </c>
+      <c r="C2455" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2455">
+        <v>1.120625</v>
+      </c>
+      <c r="O2455" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2456" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2456" t="s">
+        <v>769</v>
+      </c>
+      <c r="B2456">
+        <v>126.0027611</v>
+      </c>
+      <c r="C2456" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2456">
+        <v>22.280999999999999</v>
+      </c>
+      <c r="O2456" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2457" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2457" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2457">
+        <v>129.25714919999999</v>
+      </c>
+      <c r="C2457" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2457">
+        <v>13.042</v>
+      </c>
+      <c r="O2457" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2458" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2458" t="s">
+        <v>770</v>
+      </c>
+      <c r="B2458">
+        <v>428.41851294999998</v>
+      </c>
+      <c r="C2458" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2458">
+        <v>3.6995</v>
+      </c>
+      <c r="O2458" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2459" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2459" t="s">
+        <v>771</v>
+      </c>
+      <c r="B2459">
+        <v>161.72242360000001</v>
+      </c>
+      <c r="C2459" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2459">
+        <v>10.419</v>
+      </c>
+      <c r="O2459" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2460" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2460" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2460">
+        <v>122.3707656</v>
+      </c>
+      <c r="C2460" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2460">
+        <v>2.605</v>
+      </c>
+      <c r="O2460" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2461" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2461" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2461">
+        <v>105.2503171</v>
+      </c>
+      <c r="C2461" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2461">
+        <v>3.7919999999999998</v>
+      </c>
+      <c r="O2461" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2462" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2462" t="s">
+        <v>772</v>
+      </c>
+      <c r="B2462">
+        <v>82.670448109999995</v>
+      </c>
+      <c r="C2462" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2462">
+        <v>11.727</v>
+      </c>
+      <c r="O2462" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2463" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2463" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2463">
+        <v>147.15747020000001</v>
+      </c>
+      <c r="C2463" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2463">
+        <v>27.856999999999999</v>
+      </c>
+      <c r="O2463" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2464" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2464" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2464">
+        <v>147.638681166667</v>
+      </c>
+      <c r="C2464" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2464">
+        <v>50.127333333333297</v>
+      </c>
+      <c r="O2464" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2465" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2465" t="s">
+        <v>773</v>
+      </c>
+      <c r="B2465">
+        <v>118.50886464</v>
+      </c>
+      <c r="C2465" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2465">
+        <v>19.557200000000002</v>
+      </c>
+      <c r="O2465" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2466" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2466" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2466">
+        <v>156.8643903</v>
+      </c>
+      <c r="C2466" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2466">
+        <v>14.6436666666667</v>
+      </c>
+      <c r="O2466" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2467" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2467" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2467">
+        <v>168.23078659999999</v>
+      </c>
+      <c r="C2467" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2467">
+        <v>23.583666666666701</v>
+      </c>
+      <c r="O2467" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2468" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2468" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2468">
+        <v>105.40664538666699</v>
+      </c>
+      <c r="C2468" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2468">
+        <v>30.652333333333299</v>
+      </c>
+      <c r="O2468" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2469" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2469" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2469">
+        <v>172.62669099999999</v>
+      </c>
+      <c r="C2469" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2469">
+        <v>9.3077500000000004</v>
+      </c>
+      <c r="O2469" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2470" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2470" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2470">
+        <v>191.538969866667</v>
+      </c>
+      <c r="C2470" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2470">
+        <v>11.512</v>
+      </c>
+      <c r="O2470" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2471" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2471" t="s">
+        <v>774</v>
+      </c>
+      <c r="B2471">
+        <v>163.076491766667</v>
+      </c>
+      <c r="C2471" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2471">
+        <v>15.3693333333333</v>
+      </c>
+      <c r="O2471" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2472" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2472" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2472">
+        <v>201.25228412000001</v>
+      </c>
+      <c r="C2472" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2472">
+        <v>20.555199999999999</v>
+      </c>
+      <c r="O2472" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2473" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2473" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2473">
+        <v>238.60627568000001</v>
+      </c>
+      <c r="C2473" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2473">
+        <v>10.758599999999999</v>
+      </c>
+      <c r="O2473" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2474" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2474" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2474">
+        <v>144.79070354999999</v>
+      </c>
+      <c r="C2474" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2474">
+        <v>28.242000000000001</v>
+      </c>
+      <c r="O2474" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2475" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2475" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2475">
+        <v>164.46775410000001</v>
+      </c>
+      <c r="C2475" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2475">
+        <v>11.128</v>
+      </c>
+      <c r="O2475" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2476" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2476" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2476">
+        <v>106.271624</v>
+      </c>
+      <c r="C2476" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2476">
+        <v>14.776999999999999</v>
+      </c>
+      <c r="O2476" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2477" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2477" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2477">
+        <v>323.79513785</v>
+      </c>
+      <c r="C2477" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2477">
+        <v>34.582999999999998</v>
+      </c>
+      <c r="O2477" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2478" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2478" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2478">
+        <v>164.36722589999999</v>
+      </c>
+      <c r="C2478" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2478">
+        <v>14.041600000000001</v>
+      </c>
+      <c r="O2478" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2479" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2479" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2479">
+        <v>193.43019459999999</v>
+      </c>
+      <c r="C2479" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2479">
+        <v>51.384</v>
+      </c>
+      <c r="O2479" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2480" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2480" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2480">
+        <v>119.12951215</v>
+      </c>
+      <c r="C2480" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2480">
+        <v>55.9465</v>
+      </c>
+      <c r="O2480" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2481" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2481" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2481">
+        <v>193.16735165</v>
+      </c>
+      <c r="C2481" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2481">
+        <v>26.380749999999999</v>
+      </c>
+      <c r="O2481" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2482" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2482" t="s">
+        <v>775</v>
+      </c>
+      <c r="B2482">
+        <v>103.8166488825</v>
+      </c>
+      <c r="C2482" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2482">
+        <v>26.395250000000001</v>
+      </c>
+      <c r="O2482" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2483" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2483" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2483">
+        <v>120.91160549999999</v>
+      </c>
+      <c r="C2483" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2483">
+        <v>71.423000000000002</v>
+      </c>
+      <c r="O2483" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2484" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2484" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2484">
+        <v>132.010114566667</v>
+      </c>
+      <c r="C2484" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2484">
+        <v>60.966333333333303</v>
+      </c>
+      <c r="O2484" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2485" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2485" t="s">
+        <v>776</v>
+      </c>
+      <c r="B2485">
+        <v>165.04077955</v>
+      </c>
+      <c r="C2485" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2485">
+        <v>46.345999999999997</v>
+      </c>
+      <c r="O2485" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2486" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2486" t="s">
+        <v>775</v>
+      </c>
+      <c r="B2486">
+        <v>123.75611585</v>
+      </c>
+      <c r="C2486" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2486">
+        <v>30.3035</v>
+      </c>
+      <c r="O2486" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2487" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2487" t="s">
+        <v>769</v>
+      </c>
+      <c r="B2487">
+        <v>136.04676230000001</v>
+      </c>
+      <c r="C2487" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2487">
+        <v>27.192</v>
+      </c>
+      <c r="O2487" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2488" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2488" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2488">
+        <v>205.68262491666701</v>
+      </c>
+      <c r="C2488" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2488">
+        <v>17.446166666666699</v>
+      </c>
+      <c r="O2488" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2489" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2489" t="s">
+        <v>774</v>
+      </c>
+      <c r="B2489">
+        <v>152.70593994999999</v>
+      </c>
+      <c r="C2489" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2489">
+        <v>17.28425</v>
+      </c>
+      <c r="O2489" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2490" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2490" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2490">
+        <v>146.61406528000001</v>
+      </c>
+      <c r="C2490" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2490">
+        <v>38.432600000000001</v>
+      </c>
+      <c r="O2490" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2491" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2491" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2491">
+        <v>176.30557730000001</v>
+      </c>
+      <c r="C2491" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2491">
+        <v>21.059000000000001</v>
+      </c>
+      <c r="O2491" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2492" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2492" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2492">
+        <v>263.57163850000001</v>
+      </c>
+      <c r="C2492" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2492">
+        <v>26.658999999999999</v>
+      </c>
+      <c r="O2492" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2493" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2493" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2493">
+        <v>158.51083969999999</v>
+      </c>
+      <c r="C2493" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2493">
+        <v>10.4873333333333</v>
+      </c>
+      <c r="O2493" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2494" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2494" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2494">
+        <v>170.60176480000001</v>
+      </c>
+      <c r="C2494" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2494">
+        <v>28.557500000000001</v>
+      </c>
+      <c r="O2494" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2495" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2495" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2495">
+        <v>163.07323690000001</v>
+      </c>
+      <c r="C2495" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2495">
+        <v>56.247</v>
+      </c>
+      <c r="O2495" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2496" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2496" t="s">
+        <v>776</v>
+      </c>
+      <c r="B2496">
+        <v>172.63991390000001</v>
+      </c>
+      <c r="C2496" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2496">
+        <v>80.784000000000006</v>
+      </c>
+      <c r="O2496" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2497" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2497" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2497">
+        <v>77.289330699999994</v>
+      </c>
+      <c r="C2497" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2497">
+        <v>2.0640000000000001</v>
+      </c>
+      <c r="O2497" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2498" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2498" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2498">
+        <v>392.06720165000002</v>
+      </c>
+      <c r="C2498" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2498">
+        <v>8.2759999999999998</v>
+      </c>
+      <c r="O2498" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2499" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2499" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2499">
+        <v>156.4193578</v>
+      </c>
+      <c r="C2499" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2499">
+        <v>41.381</v>
+      </c>
+      <c r="O2499" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="2500" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2500" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2500">
+        <v>123.2354931</v>
+      </c>
+      <c r="C2500" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2500">
+        <v>43.235999999999997</v>
+      </c>
+      <c r="O2500" t="s">
+        <v>768</v>
       </c>
     </row>
   </sheetData>

</xml_diff>